<commit_message>
Word unit training added
word unit training example
give argument of
-exam_unit='word'
</commit_message>
<xml_diff>
--- a/연구노트/MorpComp 실험.xlsx
+++ b/연구노트/MorpComp 실험.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="135">
   <si>
     <t>실험명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -519,6 +519,50 @@
   </si>
   <si>
     <t>2m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>exam_unit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mbtestSGD07</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>45022 words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SGD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>word</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10secs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3646-&gt;0.2084</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mbtestSGD07</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>904462 words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8166 (1) -&gt;0.0608 (10)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1036,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1048,20 +1092,20 @@
     <col min="3" max="3" width="6.625" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="9.25" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="5.875" customWidth="1"/>
-    <col min="10" max="10" width="6" customWidth="1"/>
-    <col min="11" max="11" width="5.625" customWidth="1"/>
-    <col min="12" max="12" width="19.625" customWidth="1"/>
-    <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="14.125" customWidth="1"/>
-    <col min="15" max="15" width="20.75" customWidth="1"/>
-    <col min="16" max="16" width="17.625" customWidth="1"/>
+    <col min="6" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="9.25" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="5.875" customWidth="1"/>
+    <col min="11" max="11" width="6" customWidth="1"/>
+    <col min="12" max="12" width="5.625" customWidth="1"/>
+    <col min="13" max="13" width="19.625" customWidth="1"/>
+    <col min="14" max="14" width="28" customWidth="1"/>
+    <col min="15" max="15" width="14.125" customWidth="1"/>
+    <col min="16" max="16" width="20.75" customWidth="1"/>
+    <col min="17" max="17" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1081,37 +1125,40 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1128,32 +1175,33 @@
       <c r="F2" s="6">
         <v>0.01</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6">
         <v>30</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>32</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="6">
         <v>64</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6">
+      <c r="M2" s="6"/>
+      <c r="N2" s="6">
         <v>0.78480000000000005</v>
       </c>
-      <c r="N2" s="8">
+      <c r="O2" s="8">
         <v>0</v>
       </c>
-      <c r="O2" s="8"/>
       <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1172,32 +1220,33 @@
       <c r="F3" s="2">
         <v>0.01</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
         <v>10</v>
-      </c>
-      <c r="H3" s="2">
-        <v>300</v>
       </c>
       <c r="I3" s="2">
         <v>300</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>15</v>
+      <c r="J3" s="2">
+        <v>300</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2">
+      <c r="L3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2">
         <v>0</v>
       </c>
-      <c r="N3" s="9">
+      <c r="O3" s="9">
         <v>0.15620000000000001</v>
       </c>
-      <c r="O3" s="9"/>
       <c r="P3" s="9"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -1216,32 +1265,33 @@
       <c r="F4" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
         <v>10</v>
-      </c>
-      <c r="H4" s="2">
-        <v>300</v>
       </c>
       <c r="I4" s="2">
         <v>300</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="2">
+        <v>300</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1260,34 +1310,35 @@
       <c r="F5" s="2">
         <v>0.01</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
         <v>20</v>
-      </c>
-      <c r="H5" s="2">
-        <v>300</v>
       </c>
       <c r="I5" s="2">
         <v>300</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="2">
+        <v>300</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="9">
+      <c r="O5" s="9">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="O5" s="9"/>
       <c r="P5" s="9"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1306,34 +1357,35 @@
       <c r="F6" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
         <v>20</v>
-      </c>
-      <c r="H6" s="2">
-        <v>300</v>
       </c>
       <c r="I6" s="2">
         <v>300</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="2">
+        <v>300</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="9">
+      <c r="O6" s="9">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="O6" s="9"/>
       <c r="P6" s="9"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6" s="9"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1352,32 +1404,33 @@
       <c r="F7" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
         <v>20</v>
-      </c>
-      <c r="H7" s="2">
-        <v>300</v>
       </c>
       <c r="I7" s="2">
         <v>300</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>25</v>
+      <c r="J7" s="2">
+        <v>300</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1396,30 +1449,31 @@
       <c r="F8" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
         <v>20</v>
-      </c>
-      <c r="H8" s="2">
-        <v>300</v>
       </c>
       <c r="I8" s="2">
         <v>300</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>25</v>
+      <c r="J8" s="2">
+        <v>300</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1438,32 +1492,33 @@
       <c r="F9" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
         <v>20</v>
-      </c>
-      <c r="H9" s="2">
-        <v>300</v>
       </c>
       <c r="I9" s="2">
         <v>300</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="2">
+        <v>300</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1482,36 +1537,37 @@
       <c r="F10" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
         <v>20</v>
-      </c>
-      <c r="H10" s="2">
-        <v>300</v>
       </c>
       <c r="I10" s="2">
         <v>300</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="2">
+        <v>300</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N10" s="9">
+      <c r="O10" s="9">
         <v>0.38479999999999998</v>
       </c>
-      <c r="O10" s="9"/>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="9"/>
+      <c r="Q10" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -1530,36 +1586,37 @@
       <c r="F11" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
         <v>20</v>
-      </c>
-      <c r="H11" s="2">
-        <v>300</v>
       </c>
       <c r="I11" s="2">
         <v>300</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="2">
+        <v>300</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N11" s="9">
+      <c r="O11" s="9">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="O11" s="9"/>
-      <c r="P11" s="2" t="s">
+      <c r="P11" s="9"/>
+      <c r="Q11" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
@@ -1578,34 +1635,35 @@
       <c r="F12" s="2">
         <v>1E-3</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2">
         <v>30</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>128</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>256</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>56</v>
       </c>
       <c r="L12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="N12" s="9"/>
       <c r="O12" s="9"/>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="9"/>
+      <c r="Q12" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -1624,32 +1682,33 @@
       <c r="F13" s="11">
         <v>1E-3</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="11"/>
+      <c r="H13" s="2">
         <v>30</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>128</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>256</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>56</v>
       </c>
       <c r="L13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="12">
+      <c r="N13" s="2"/>
+      <c r="O13" s="12">
         <v>0</v>
       </c>
-      <c r="O13" s="12"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P13" s="12"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>61</v>
       </c>
@@ -1668,34 +1727,35 @@
       <c r="F14" s="11">
         <v>0.01</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="11"/>
+      <c r="H14" s="2">
         <v>30</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>128</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>256</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>56</v>
       </c>
       <c r="L14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="N14" s="12">
+      <c r="O14" s="12">
         <v>1</v>
       </c>
-      <c r="O14" s="12"/>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P14" s="12"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
@@ -1714,32 +1774,33 @@
       <c r="F15" s="11">
         <v>0.01</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="11"/>
+      <c r="H15" s="2">
         <v>30</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>128</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>256</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="12"/>
       <c r="O15" s="12"/>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P15" s="12"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>75</v>
       </c>
@@ -1758,32 +1819,33 @@
       <c r="F16" s="2">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2">
         <v>30</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>128</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>256</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>83</v>
       </c>
@@ -1802,34 +1864,35 @@
       <c r="F17" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2">
         <v>15</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>128</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>256</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>86</v>
       </c>
       <c r="L17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="N17" s="9">
+      <c r="O17" s="9">
         <v>0.37040000000000001</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P17" s="9"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>89</v>
       </c>
@@ -1848,34 +1911,35 @@
       <c r="F18" s="2">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2">
         <v>15</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>128</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>256</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>86</v>
       </c>
       <c r="L18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="N18" s="9">
+      <c r="O18" s="9">
         <v>0.5887</v>
       </c>
-      <c r="O18" s="9"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P18" s="9"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>94</v>
       </c>
@@ -1894,38 +1958,39 @@
       <c r="F19" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2">
         <v>20</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>128</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>256</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>86</v>
       </c>
       <c r="L19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N19" s="13">
+      <c r="O19" s="13">
         <v>0.99590000000000001</v>
       </c>
-      <c r="O19" s="13">
+      <c r="P19" s="13">
         <v>0.13</v>
       </c>
-      <c r="P19" s="2" t="s">
+      <c r="Q19" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>107</v>
       </c>
@@ -1944,34 +2009,35 @@
       <c r="F20" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2">
         <v>24</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>256</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>512</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="9" t="s">
+      <c r="O20" s="2"/>
+      <c r="P20" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>99</v>
       </c>
@@ -1990,34 +2056,35 @@
       <c r="F21" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2">
         <v>24</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>256</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>512</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="N21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="9" t="s">
+      <c r="O21" s="2"/>
+      <c r="P21" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="P21" s="2"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>111</v>
       </c>
@@ -2036,34 +2103,35 @@
       <c r="F22" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2">
         <v>24</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>256</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>512</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="N22" s="2"/>
-      <c r="O22" s="9">
+      <c r="O22" s="2"/>
+      <c r="P22" s="9">
         <v>0.4052</v>
       </c>
-      <c r="P22" s="2"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>119</v>
       </c>
@@ -2082,54 +2150,92 @@
       <c r="F23" s="2">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2">
         <v>24</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>256</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>512</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="9">
+      <c r="O23" s="2"/>
+      <c r="P23" s="9">
         <v>0.50890000000000002</v>
       </c>
-      <c r="P23" s="2"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="2">
+        <v>128</v>
+      </c>
+      <c r="D24" s="2">
+        <v>100</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="2">
+        <v>10</v>
+      </c>
+      <c r="I24" s="2">
+        <v>256</v>
+      </c>
+      <c r="J24" s="2">
+        <v>512</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="2">
+        <v>128</v>
+      </c>
+      <c r="D25" s="2">
+        <v>100</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2139,11 +2245,14 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+      <c r="N25" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2160,8 +2269,9 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2178,8 +2288,9 @@
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2196,8 +2307,9 @@
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2214,8 +2326,9 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2232,8 +2345,9 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2250,8 +2364,9 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2268,8 +2383,9 @@
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2286,8 +2402,9 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q33" s="1"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2304,8 +2421,9 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q34" s="1"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2322,8 +2440,9 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q35" s="1"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2340,8 +2459,9 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q36" s="1"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2358,8 +2478,9 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q37" s="1"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2376,8 +2497,9 @@
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q38" s="1"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2394,8 +2516,9 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q39" s="1"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2412,8 +2535,9 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2430,6 +2554,7 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Test data management added
1. add trained data to the ../data/test/ directory with model name
2. from that information, choose
 closed_test, test data sets
3. all reflected on the Evaluation.py
</commit_message>
<xml_diff>
--- a/연구노트/MorpComp 실험.xlsx
+++ b/연구노트/MorpComp 실험.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="170">
   <si>
     <t>실험명</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -563,6 +563,146 @@
   </si>
   <si>
     <t>0.8166 (1) -&gt;0.0608 (10)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mbtestSGD08</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>outta 168189 words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SGD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>word</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>75 mins</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1834700 words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1912 (1) -&gt; 0.0045 (20)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.71%(167863 words)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mbtestSGD08-16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SGD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>word</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>24 mins</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1829357 words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mbtestSGD09</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1836386 words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>morp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>word</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SGD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>25 mins</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.7484 (1) -&gt; 0.1255 (20)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>95.01% (159023 words)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>outta 167377 words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>152411 문장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mbtestSGD10-12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SGD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>word</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syll</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1796784 words</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>18 mins</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9793 (1) -&gt; 0.0096 (50)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -753,7 +893,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -797,6 +937,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1080,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1101,7 +1244,7 @@
     <col min="13" max="13" width="19.625" customWidth="1"/>
     <col min="14" max="14" width="28" customWidth="1"/>
     <col min="15" max="15" width="14.125" customWidth="1"/>
-    <col min="16" max="16" width="20.75" customWidth="1"/>
+    <col min="16" max="16" width="26.25" customWidth="1"/>
     <col min="17" max="17" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1845,7 +1988,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>83</v>
       </c>
@@ -1892,7 +2035,7 @@
       <c r="P17" s="9"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>89</v>
       </c>
@@ -1939,7 +2082,7 @@
       <c r="P18" s="9"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>94</v>
       </c>
@@ -1990,7 +2133,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>107</v>
       </c>
@@ -2037,7 +2180,7 @@
       </c>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>99</v>
       </c>
@@ -2084,7 +2227,7 @@
       </c>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>111</v>
       </c>
@@ -2131,7 +2274,7 @@
       </c>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>119</v>
       </c>
@@ -2176,7 +2319,7 @@
       </c>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>125</v>
       </c>
@@ -2223,7 +2366,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>132</v>
       </c>
@@ -2252,83 +2395,210 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="11">
+        <v>20</v>
+      </c>
+      <c r="D26" s="2">
+        <v>20</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H26" s="2">
+        <v>20</v>
+      </c>
+      <c r="I26" s="2">
+        <v>256</v>
+      </c>
+      <c r="J26" s="2">
+        <v>512</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O26" s="15">
+        <v>0.97</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R26" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C27" s="11">
+        <v>128</v>
+      </c>
+      <c r="D27" s="2">
+        <v>20</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H27" s="2">
+        <v>16</v>
+      </c>
+      <c r="I27" s="2">
+        <v>256</v>
+      </c>
+      <c r="J27" s="2">
+        <v>512</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
+      <c r="O27" s="15">
+        <v>0.93</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="2">
+        <v>128</v>
+      </c>
+      <c r="D28" s="2">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" s="2">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2">
+        <v>256</v>
+      </c>
+      <c r="J28" s="2">
+        <v>512</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O28" s="9">
+        <v>0.67820000000000003</v>
+      </c>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="2">
+        <v>128</v>
+      </c>
+      <c r="D29" s="2">
+        <v>50</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F29" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H29" s="2">
+        <v>12</v>
+      </c>
+      <c r="I29" s="2">
+        <v>256</v>
+      </c>
+      <c r="J29" s="2">
+        <v>512</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2347,7 +2617,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2366,7 +2636,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>

</xml_diff>